<commit_message>
Making final changes to correct_program_runner.py
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -7,8 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="All Results" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Summary" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="All Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Minimum Values" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18,16 +18,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -38,7 +35,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -46,21 +43,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -426,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,72 +423,72 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>input_file</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>output_file</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>trial</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>serial_timesteps</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>serial_timetaken</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>parallel_timesteps</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>parallel_timetaken</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>is_correct</t>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>image_similarity</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>8_by_8_all_4.csv</t>
+          <t>32_by_32_all_8.csv</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>8.png</t>
+          <t>32.png</t>
         </is>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>19</v>
+        <v>512</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F2" t="n">
-        <v>19</v>
+        <v>512</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="H2" t="b">
         <v>1</v>
@@ -509,28 +497,28 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>8_by_8_all_4.csv</t>
+          <t>32_by_32_all_8.csv</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>8.png</t>
+          <t>32.png</t>
         </is>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>19</v>
+        <v>512</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F3" t="n">
-        <v>19</v>
+        <v>512</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="H3" t="b">
         <v>1</v>
@@ -539,28 +527,28 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>16_by_16_all_4.csv</t>
+          <t>32_by_32_all_8.csv</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>16.png</t>
+          <t>32.png</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D4" t="n">
-        <v>67</v>
+        <v>512</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F4" t="n">
-        <v>67</v>
+        <v>512</v>
       </c>
       <c r="G4" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="H4" t="b">
         <v>1</v>
@@ -569,28 +557,28 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>16_by_16_all_4.csv</t>
+          <t>32_by_32_all_8.csv</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>16.png</t>
+          <t>32.png</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D5" t="n">
-        <v>67</v>
+        <v>512</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>67</v>
+        <v>512</v>
       </c>
       <c r="G5" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="H5" t="b">
         <v>1</v>
@@ -599,28 +587,28 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>16_by_16_one_100.csv</t>
+          <t>32_by_32_all_8.csv</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16One.png</t>
+          <t>32.png</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D6" t="n">
-        <v>19</v>
+        <v>512</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F6" t="n">
-        <v>19</v>
+        <v>512</v>
       </c>
       <c r="G6" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="H6" t="b">
         <v>1</v>
@@ -629,30 +617,750 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>16_by_16_one_100.csv</t>
+          <t>32_by_32_all_8.csv</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16One.png</t>
+          <t>32.png</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D7" t="n">
-        <v>19</v>
+        <v>512</v>
       </c>
       <c r="E7" t="n">
+        <v>10</v>
+      </c>
+      <c r="F7" t="n">
+        <v>512</v>
+      </c>
+      <c r="G7" t="n">
+        <v>16</v>
+      </c>
+      <c r="H7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>32_by_32_all_8.csv</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>32.png</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>6</v>
+      </c>
+      <c r="D8" t="n">
+        <v>512</v>
+      </c>
+      <c r="E8" t="n">
+        <v>9</v>
+      </c>
+      <c r="F8" t="n">
+        <v>512</v>
+      </c>
+      <c r="G8" t="n">
+        <v>18</v>
+      </c>
+      <c r="H8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>32_by_32_all_8.csv</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>32.png</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>7</v>
+      </c>
+      <c r="D9" t="n">
+        <v>512</v>
+      </c>
+      <c r="E9" t="n">
+        <v>9</v>
+      </c>
+      <c r="F9" t="n">
+        <v>512</v>
+      </c>
+      <c r="G9" t="n">
+        <v>17</v>
+      </c>
+      <c r="H9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>32_by_32_all_8.csv</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>32.png</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>8</v>
+      </c>
+      <c r="D10" t="n">
+        <v>512</v>
+      </c>
+      <c r="E10" t="n">
+        <v>10</v>
+      </c>
+      <c r="F10" t="n">
+        <v>512</v>
+      </c>
+      <c r="G10" t="n">
+        <v>17</v>
+      </c>
+      <c r="H10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>32_by_32_all_8.csv</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>32.png</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>9</v>
+      </c>
+      <c r="D11" t="n">
+        <v>512</v>
+      </c>
+      <c r="E11" t="n">
+        <v>9</v>
+      </c>
+      <c r="F11" t="n">
+        <v>512</v>
+      </c>
+      <c r="G11" t="n">
+        <v>17</v>
+      </c>
+      <c r="H11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>125_by_125_center_1111.csv</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>125_center.png</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
         <v>0</v>
       </c>
-      <c r="F7" t="n">
-        <v>19</v>
-      </c>
-      <c r="G7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" t="b">
+      <c r="D12" t="n">
+        <v>5814</v>
+      </c>
+      <c r="E12" t="n">
+        <v>198</v>
+      </c>
+      <c r="F12" t="n">
+        <v>5814</v>
+      </c>
+      <c r="G12" t="n">
+        <v>349</v>
+      </c>
+      <c r="H12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>125_by_125_center_1111.csv</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>125_center.png</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" t="n">
+        <v>5814</v>
+      </c>
+      <c r="E13" t="n">
+        <v>199</v>
+      </c>
+      <c r="F13" t="n">
+        <v>5814</v>
+      </c>
+      <c r="G13" t="n">
+        <v>332</v>
+      </c>
+      <c r="H13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>125_by_125_center_1111.csv</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>125_center.png</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" t="n">
+        <v>5814</v>
+      </c>
+      <c r="E14" t="n">
+        <v>198</v>
+      </c>
+      <c r="F14" t="n">
+        <v>5814</v>
+      </c>
+      <c r="G14" t="n">
+        <v>340</v>
+      </c>
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>125_by_125_center_1111.csv</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>125_center.png</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>3</v>
+      </c>
+      <c r="D15" t="n">
+        <v>5814</v>
+      </c>
+      <c r="E15" t="n">
+        <v>195</v>
+      </c>
+      <c r="F15" t="n">
+        <v>5814</v>
+      </c>
+      <c r="G15" t="n">
+        <v>347</v>
+      </c>
+      <c r="H15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>125_by_125_center_1111.csv</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>125_center.png</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>4</v>
+      </c>
+      <c r="D16" t="n">
+        <v>5814</v>
+      </c>
+      <c r="E16" t="n">
+        <v>196</v>
+      </c>
+      <c r="F16" t="n">
+        <v>5814</v>
+      </c>
+      <c r="G16" t="n">
+        <v>356</v>
+      </c>
+      <c r="H16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>125_by_125_center_1111.csv</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>125_center.png</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>5</v>
+      </c>
+      <c r="D17" t="n">
+        <v>5814</v>
+      </c>
+      <c r="E17" t="n">
+        <v>196</v>
+      </c>
+      <c r="F17" t="n">
+        <v>5814</v>
+      </c>
+      <c r="G17" t="n">
+        <v>338</v>
+      </c>
+      <c r="H17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>125_by_125_center_1111.csv</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>125_center.png</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>6</v>
+      </c>
+      <c r="D18" t="n">
+        <v>5814</v>
+      </c>
+      <c r="E18" t="n">
+        <v>195</v>
+      </c>
+      <c r="F18" t="n">
+        <v>5814</v>
+      </c>
+      <c r="G18" t="n">
+        <v>340</v>
+      </c>
+      <c r="H18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>125_by_125_center_1111.csv</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>125_center.png</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>7</v>
+      </c>
+      <c r="D19" t="n">
+        <v>5814</v>
+      </c>
+      <c r="E19" t="n">
+        <v>204</v>
+      </c>
+      <c r="F19" t="n">
+        <v>5814</v>
+      </c>
+      <c r="G19" t="n">
+        <v>358</v>
+      </c>
+      <c r="H19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>125_by_125_center_1111.csv</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>125_center.png</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>8</v>
+      </c>
+      <c r="D20" t="n">
+        <v>5814</v>
+      </c>
+      <c r="E20" t="n">
+        <v>200</v>
+      </c>
+      <c r="F20" t="n">
+        <v>5814</v>
+      </c>
+      <c r="G20" t="n">
+        <v>340</v>
+      </c>
+      <c r="H20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>125_by_125_center_1111.csv</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>125_center.png</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>9</v>
+      </c>
+      <c r="D21" t="n">
+        <v>5814</v>
+      </c>
+      <c r="E21" t="n">
+        <v>204</v>
+      </c>
+      <c r="F21" t="n">
+        <v>5814</v>
+      </c>
+      <c r="G21" t="n">
+        <v>332</v>
+      </c>
+      <c r="H21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>750_by_750_center_777.csv</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>750_777.png</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>133</v>
+      </c>
+      <c r="E22" t="n">
+        <v>170</v>
+      </c>
+      <c r="F22" t="n">
+        <v>133</v>
+      </c>
+      <c r="G22" t="n">
+        <v>62</v>
+      </c>
+      <c r="H22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>750_by_750_center_777.csv</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>750_777.png</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" t="n">
+        <v>133</v>
+      </c>
+      <c r="E23" t="n">
+        <v>175</v>
+      </c>
+      <c r="F23" t="n">
+        <v>133</v>
+      </c>
+      <c r="G23" t="n">
+        <v>60</v>
+      </c>
+      <c r="H23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>750_by_750_center_777.csv</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>750_777.png</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>2</v>
+      </c>
+      <c r="D24" t="n">
+        <v>133</v>
+      </c>
+      <c r="E24" t="n">
+        <v>170</v>
+      </c>
+      <c r="F24" t="n">
+        <v>133</v>
+      </c>
+      <c r="G24" t="n">
+        <v>69</v>
+      </c>
+      <c r="H24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>750_by_750_center_777.csv</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>750_777.png</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>3</v>
+      </c>
+      <c r="D25" t="n">
+        <v>133</v>
+      </c>
+      <c r="E25" t="n">
+        <v>163</v>
+      </c>
+      <c r="F25" t="n">
+        <v>133</v>
+      </c>
+      <c r="G25" t="n">
+        <v>65</v>
+      </c>
+      <c r="H25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>750_by_750_center_777.csv</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>750_777.png</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>4</v>
+      </c>
+      <c r="D26" t="n">
+        <v>133</v>
+      </c>
+      <c r="E26" t="n">
+        <v>169</v>
+      </c>
+      <c r="F26" t="n">
+        <v>133</v>
+      </c>
+      <c r="G26" t="n">
+        <v>64</v>
+      </c>
+      <c r="H26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>750_by_750_center_777.csv</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>750_777.png</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>5</v>
+      </c>
+      <c r="D27" t="n">
+        <v>133</v>
+      </c>
+      <c r="E27" t="n">
+        <v>183</v>
+      </c>
+      <c r="F27" t="n">
+        <v>133</v>
+      </c>
+      <c r="G27" t="n">
+        <v>60</v>
+      </c>
+      <c r="H27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>750_by_750_center_777.csv</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>750_777.png</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>6</v>
+      </c>
+      <c r="D28" t="n">
+        <v>133</v>
+      </c>
+      <c r="E28" t="n">
+        <v>175</v>
+      </c>
+      <c r="F28" t="n">
+        <v>133</v>
+      </c>
+      <c r="G28" t="n">
+        <v>66</v>
+      </c>
+      <c r="H28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>750_by_750_center_777.csv</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>750_777.png</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>7</v>
+      </c>
+      <c r="D29" t="n">
+        <v>133</v>
+      </c>
+      <c r="E29" t="n">
+        <v>172</v>
+      </c>
+      <c r="F29" t="n">
+        <v>133</v>
+      </c>
+      <c r="G29" t="n">
+        <v>66</v>
+      </c>
+      <c r="H29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>750_by_750_center_777.csv</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>750_777.png</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>8</v>
+      </c>
+      <c r="D30" t="n">
+        <v>133</v>
+      </c>
+      <c r="E30" t="n">
+        <v>180</v>
+      </c>
+      <c r="F30" t="n">
+        <v>133</v>
+      </c>
+      <c r="G30" t="n">
+        <v>59</v>
+      </c>
+      <c r="H30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>750_by_750_center_777.csv</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>750_777.png</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>9</v>
+      </c>
+      <c r="D31" t="n">
+        <v>133</v>
+      </c>
+      <c r="E31" t="n">
+        <v>173</v>
+      </c>
+      <c r="F31" t="n">
+        <v>133</v>
+      </c>
+      <c r="G31" t="n">
+        <v>60</v>
+      </c>
+      <c r="H31" t="b">
         <v>1</v>
       </c>
     </row>
@@ -676,37 +1384,37 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>input_file</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>output_file</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>serial_timesteps</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>serial_timetaken</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>parallel_timesteps</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>parallel_timetaken</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>correctness_rate</t>
         </is>
@@ -715,25 +1423,25 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>16_by_16_all_4.csv</t>
+          <t>125_by_125_center_1111.csv</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>16.png</t>
+          <t>125_center.png</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>67</v>
+        <v>5814</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>195</v>
       </c>
       <c r="E2" t="n">
-        <v>67</v>
+        <v>5814</v>
       </c>
       <c r="F2" t="n">
-        <v>3</v>
+        <v>332</v>
       </c>
       <c r="G2" t="n">
         <v>1</v>
@@ -742,25 +1450,25 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>16_by_16_one_100.csv</t>
+          <t>32_by_32_all_8.csv</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>16One.png</t>
+          <t>32.png</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>19</v>
+        <v>512</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E3" t="n">
-        <v>19</v>
+        <v>512</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G3" t="n">
         <v>1</v>
@@ -769,25 +1477,25 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>8_by_8_all_4.csv</t>
+          <t>750_by_750_center_777.csv</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>8.png</t>
+          <t>750_777.png</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>19</v>
+        <v>133</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>163</v>
       </c>
       <c r="E4" t="n">
-        <v>19</v>
+        <v>133</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="G4" t="n">
         <v>1</v>

</xml_diff>